<commit_message>
Updated README file, improved the workflow, added Douro map with municipalities and some of wine producers
</commit_message>
<xml_diff>
--- a/data_source/douro/douro_municipality_parish.xlsx
+++ b/data_source/douro/douro_municipality_parish.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GIS_Master\Semester2\EGM722\Assigment\wine_project\data_source\douro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255202DE-1F07-40A6-898E-2C194DA74FEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4D2405-517C-4099-9873-EFA7BDE09ABA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5115" yWindow="645" windowWidth="15375" windowHeight="10095" xr2:uid="{4777063A-2C50-4CED-AB95-4D3D8DD05213}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="134">
   <si>
     <t>Baxio Corgo</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Vilarinho de São Romão</t>
   </si>
   <si>
-    <t>S. João da Pesqueira</t>
-  </si>
-  <si>
     <t>Casais do Douro</t>
   </si>
   <si>
@@ -405,9 +402,6 @@
     <t>Vilas Boas</t>
   </si>
   <si>
-    <t>Figueira Castelo Rodrigo</t>
-  </si>
-  <si>
     <t>Escalhão</t>
   </si>
   <si>
@@ -433,6 +427,15 @@
   </si>
   <si>
     <t>Santa Marta de Penaguião</t>
+  </si>
+  <si>
+    <t>Mêda</t>
+  </si>
+  <si>
+    <t>Freixo de Espada À Cinta</t>
+  </si>
+  <si>
+    <t>Figueira de Castelo Rodrigo</t>
   </si>
 </sst>
 </file>
@@ -794,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38ECEDF1-4017-4228-B26A-DC2A4C856958}">
   <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -821,7 +824,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -829,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -837,7 +840,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1494,10 +1497,10 @@
         <v>36</v>
       </c>
       <c r="B64" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" t="s">
         <v>67</v>
-      </c>
-      <c r="C64" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1505,10 +1508,10 @@
         <v>36</v>
       </c>
       <c r="B65" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1516,10 +1519,10 @@
         <v>36</v>
       </c>
       <c r="B66" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1527,10 +1530,10 @@
         <v>36</v>
       </c>
       <c r="B67" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1538,10 +1541,10 @@
         <v>36</v>
       </c>
       <c r="B68" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1549,10 +1552,10 @@
         <v>36</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1560,10 +1563,10 @@
         <v>36</v>
       </c>
       <c r="B70" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1571,10 +1574,10 @@
         <v>36</v>
       </c>
       <c r="B71" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1582,10 +1585,10 @@
         <v>36</v>
       </c>
       <c r="B72" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C72" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1593,10 +1596,10 @@
         <v>36</v>
       </c>
       <c r="B73" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C73" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1604,10 +1607,10 @@
         <v>36</v>
       </c>
       <c r="B74" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C74" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1615,10 +1618,10 @@
         <v>36</v>
       </c>
       <c r="B75" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1626,10 +1629,10 @@
         <v>36</v>
       </c>
       <c r="B76" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C76" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1637,10 +1640,10 @@
         <v>36</v>
       </c>
       <c r="B77" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C77" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1648,10 +1651,10 @@
         <v>36</v>
       </c>
       <c r="B78" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78" t="s">
         <v>82</v>
-      </c>
-      <c r="C78" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1659,10 +1662,10 @@
         <v>36</v>
       </c>
       <c r="B79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C79" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1670,10 +1673,10 @@
         <v>36</v>
       </c>
       <c r="B80" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C80" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1681,10 +1684,10 @@
         <v>36</v>
       </c>
       <c r="B81" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1692,10 +1695,10 @@
         <v>36</v>
       </c>
       <c r="B82" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C82" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1703,10 +1706,10 @@
         <v>36</v>
       </c>
       <c r="B83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C83" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1714,10 +1717,10 @@
         <v>36</v>
       </c>
       <c r="B84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C84" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1725,10 +1728,10 @@
         <v>36</v>
       </c>
       <c r="B85" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C85" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1736,10 +1739,10 @@
         <v>36</v>
       </c>
       <c r="B86" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C86" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1747,381 +1750,381 @@
         <v>36</v>
       </c>
       <c r="B87" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C87" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" t="s">
         <v>92</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>93</v>
-      </c>
-      <c r="C88" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>95</v>
+        <v>132</v>
       </c>
       <c r="C89" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B90" t="s">
+        <v>132</v>
+      </c>
+      <c r="C90" t="s">
         <v>95</v>
-      </c>
-      <c r="C90" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>95</v>
+        <v>132</v>
       </c>
       <c r="C91" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>95</v>
+        <v>132</v>
       </c>
       <c r="C92" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93" t="s">
+        <v>98</v>
+      </c>
+      <c r="C93" t="s">
         <v>99</v>
-      </c>
-      <c r="C93" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B94" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C94" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C95" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B96" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C96" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B97" t="s">
+        <v>103</v>
+      </c>
+      <c r="C97" t="s">
         <v>104</v>
-      </c>
-      <c r="C97" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B98" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C98" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B99" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C99" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B100" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C100" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B101" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C101" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B102" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C102" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B103" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C103" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B104" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C104" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B105" t="s">
+        <v>111</v>
+      </c>
+      <c r="C105" t="s">
         <v>112</v>
-      </c>
-      <c r="C105" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B106" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C106" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B107" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C107" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B108" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C108" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B109" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C109" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B110" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C110" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B111" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C111" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B112" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C112" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B113" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C113" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B114" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C114" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B115" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C115" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B116" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="C116" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B117" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C117" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B118" t="s">
+        <v>131</v>
+      </c>
+      <c r="C118" t="s">
         <v>125</v>
-      </c>
-      <c r="C118" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B119" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C119" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B120" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C120" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B121" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>